<commit_message>
bug fix stats.mannwhitneyu(), add alternative=two-sided for correct p value
</commit_message>
<xml_diff>
--- a/results/celltype-specific_inferential_stats.xlsx
+++ b/results/celltype-specific_inferential_stats.xlsx
@@ -468,7 +468,7 @@
         <v>409307</v>
       </c>
       <c r="H2">
-        <v>1.32492399703841e-37</v>
+        <v>2.64984799407682e-37</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -494,7 +494,7 @@
         <v>420999</v>
       </c>
       <c r="H3">
-        <v>8.55469206969686e-30</v>
+        <v>1.710938413939372e-29</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -520,7 +520,7 @@
         <v>357621</v>
       </c>
       <c r="H4">
-        <v>1.254372935985448e-11</v>
+        <v>2.508745871970896e-11</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -546,7 +546,7 @@
         <v>107010</v>
       </c>
       <c r="H5">
-        <v>5.104470742382786e-16</v>
+        <v>1.020894148476557e-15</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -572,7 +572,7 @@
         <v>290671</v>
       </c>
       <c r="H6">
-        <v>1.420280129662831e-18</v>
+        <v>2.840560259325662e-18</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -598,7 +598,7 @@
         <v>374249</v>
       </c>
       <c r="H7">
-        <v>3.075298161544939e-36</v>
+        <v>6.150596323089877e-36</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -624,7 +624,7 @@
         <v>358063</v>
       </c>
       <c r="H8">
-        <v>1.142849167349756e-40</v>
+        <v>2.285698334699512e-40</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -650,7 +650,7 @@
         <v>536949</v>
       </c>
       <c r="H9">
-        <v>3.277296324747267e-43</v>
+        <v>6.554592649494534e-43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
check whether using celltyp-expressed genes instead of celltype-specific genes would change the results
</commit_message>
<xml_diff>
--- a/results/celltype-specific_inferential_stats.xlsx
+++ b/results/celltype-specific_inferential_stats.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_E49A4393E197E304B40A2453F42D62B100BF7491" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1516D99-0674-0442-A077-FEFA3406B1E5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28800" yWindow="-12540" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mouse reference genome" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -64,8 +70,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +134,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -174,7 +188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -206,9 +220,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -240,6 +272,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -415,14 +465,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="381" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,7 +506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -453,25 +514,25 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>212.9427806776603</v>
+        <v>212.94278067766029</v>
       </c>
       <c r="D2">
-        <v>5.75523014541824e-47</v>
+        <v>5.7552301454182397E-47</v>
       </c>
       <c r="E2">
-        <v>264.646813073132</v>
+        <v>264.64681307313202</v>
       </c>
       <c r="F2">
-        <v>4.545494287279642e-56</v>
+        <v>4.5454942872796416E-56</v>
       </c>
       <c r="G2">
         <v>409307</v>
       </c>
       <c r="H2">
-        <v>2.64984799407682e-37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>2.64984799407682E-37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -482,22 +543,22 @@
         <v>150.8220466694533</v>
       </c>
       <c r="D3">
-        <v>1.775859860493562e-33</v>
+        <v>1.7758598604935619E-33</v>
       </c>
       <c r="E3">
-        <v>229.8132839703974</v>
+        <v>229.81328397039741</v>
       </c>
       <c r="F3">
-        <v>1.44806406260533e-48</v>
+        <v>1.4480640626053299E-48</v>
       </c>
       <c r="G3">
         <v>420999</v>
       </c>
       <c r="H3">
-        <v>1.710938413939372e-29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>1.710938413939372E-29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -505,25 +566,25 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>75.07725305403983</v>
+        <v>75.077253054039829</v>
       </c>
       <c r="D4">
-        <v>4.9794530409934e-17</v>
+        <v>4.9794530409933999E-17</v>
       </c>
       <c r="E4">
-        <v>83.88310073555658</v>
+        <v>83.883100735556582</v>
       </c>
       <c r="F4">
-        <v>2.61754304933234e-17</v>
+        <v>2.61754304933234E-17</v>
       </c>
       <c r="G4">
         <v>357621</v>
       </c>
       <c r="H4">
-        <v>2.508745871970896e-11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>2.5087458719708958E-11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -531,25 +592,25 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>77.07129926896778</v>
+        <v>77.071299268967778</v>
       </c>
       <c r="D5">
-        <v>1.8372997129611e-17</v>
+        <v>1.8372997129611001E-17</v>
       </c>
       <c r="E5">
         <v>125.4235138372769</v>
       </c>
       <c r="F5">
-        <v>3.705523749947616e-26</v>
+        <v>3.7055237499476162E-26</v>
       </c>
       <c r="G5">
         <v>107010</v>
       </c>
       <c r="H5">
-        <v>1.020894148476557e-15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>1.0208941484765571E-15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -560,22 +621,22 @@
         <v>101.7846536397128</v>
       </c>
       <c r="D6">
-        <v>7.902114003114189e-23</v>
+        <v>7.9021140031141892E-23</v>
       </c>
       <c r="E6">
         <v>115.6031614179974</v>
       </c>
       <c r="F6">
-        <v>4.639609764429649e-24</v>
+        <v>4.6396097644296492E-24</v>
       </c>
       <c r="G6">
         <v>290671</v>
       </c>
       <c r="H6">
-        <v>2.840560259325662e-18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>2.840560259325662E-18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -586,22 +647,22 @@
         <v>207.2223014091123</v>
       </c>
       <c r="D7">
-        <v>1.005191911679272e-45</v>
+        <v>1.005191911679272E-45</v>
       </c>
       <c r="E7">
-        <v>256.2549008880796</v>
+        <v>256.25490088807959</v>
       </c>
       <c r="F7">
-        <v>2.92397643356789e-54</v>
+        <v>2.9239764335678902E-54</v>
       </c>
       <c r="G7">
         <v>374249</v>
       </c>
       <c r="H7">
-        <v>6.150596323089877e-36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>6.1505963230898775E-36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -612,22 +673,22 @@
         <v>226.0450761962984</v>
       </c>
       <c r="D8">
-        <v>8.221203023251265e-50</v>
+        <v>8.2212030232512655E-50</v>
       </c>
       <c r="E8">
-        <v>271.0826059002957</v>
+        <v>271.08260590029568</v>
       </c>
       <c r="F8">
-        <v>1.863906408710017e-57</v>
+        <v>1.8639064087100169E-57</v>
       </c>
       <c r="G8">
         <v>358063</v>
       </c>
       <c r="H8">
-        <v>2.285698334699512e-40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>2.2856983346995119E-40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -635,22 +696,22 @@
         <v>14</v>
       </c>
       <c r="C9">
-        <v>252.1207093062876</v>
+        <v>252.12070930628761</v>
       </c>
       <c r="D9">
-        <v>1.789301752822462e-55</v>
+        <v>1.7893017528224621E-55</v>
       </c>
       <c r="E9">
-        <v>347.2182768062976</v>
+        <v>347.21827680629758</v>
       </c>
       <c r="F9">
-        <v>6.991593225467283e-74</v>
+        <v>6.9915932254672826E-74</v>
       </c>
       <c r="G9">
         <v>536949</v>
       </c>
       <c r="H9">
-        <v>6.554592649494534e-43</v>
+        <v>6.5545926494945338E-43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update statistics and visualization for all 92 species--matching dot plot generated with JMP
</commit_message>
<xml_diff>
--- a/results/celltype-specific_inferential_stats.xlsx
+++ b/results/celltype-specific_inferential_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vanderbilt365-my.sharepoint.com/personal/linhe_xu_vanderbilt_edu/Documents/Herculano_Lab/Projects/neuron-glia-dNdS/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_E49A4393E197E304B40A2453F42D62B100BF7491" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C1516D99-0674-0442-A077-FEFA3406B1E5}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="11_2DB60FE75CC66E3E802A3FB8042C773D61B43245" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{775E7B7D-D746-CC46-B16D-04F1988EB314}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-12540" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24920" yWindow="4140" windowWidth="21580" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mouse reference genome" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Species</t>
   </si>
@@ -43,6 +43,36 @@
     <t>Mann p NG</t>
   </si>
   <si>
+    <t>Mann U NE</t>
+  </si>
+  <si>
+    <t>Mann p NE</t>
+  </si>
+  <si>
+    <t>Mann U EG</t>
+  </si>
+  <si>
+    <t>Mann p EG</t>
+  </si>
+  <si>
+    <t>Mann U NA</t>
+  </si>
+  <si>
+    <t>Mann p NA</t>
+  </si>
+  <si>
+    <t>Mann U NM</t>
+  </si>
+  <si>
+    <t>Mann p NM</t>
+  </si>
+  <si>
+    <t>Mann U NO</t>
+  </si>
+  <si>
+    <t>Mann p NO</t>
+  </si>
+  <si>
     <t>human</t>
   </si>
   <si>
@@ -64,7 +94,7 @@
     <t>pig</t>
   </si>
   <si>
-    <t>avg_93species</t>
+    <t>avg_92species</t>
   </si>
 </sst>
 </file>
@@ -466,252 +496,507 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="381" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" customWidth="1"/>
+    <col min="13" max="13" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>212.94278067766029</v>
       </c>
       <c r="C2">
-        <v>212.94278067766029</v>
+        <v>5.7552301454182397E-47</v>
       </c>
       <c r="D2">
-        <v>5.7552301454182397E-47</v>
+        <v>264.64681307313202</v>
       </c>
       <c r="E2">
-        <v>264.64681307313202</v>
+        <v>4.5454942872796416E-56</v>
       </c>
       <c r="F2">
-        <v>4.5454942872796416E-56</v>
+        <v>409307</v>
       </c>
       <c r="G2">
-        <v>409307</v>
+        <v>2.64984799407682E-37</v>
       </c>
       <c r="H2">
-        <v>2.64984799407682E-37</v>
+        <v>314600</v>
+      </c>
+      <c r="I2">
+        <v>4.862393188236875E-33</v>
+      </c>
+      <c r="J2">
+        <v>413206</v>
+      </c>
+      <c r="K2">
+        <v>0.82390759190151674</v>
+      </c>
+      <c r="L2">
+        <v>340443</v>
+      </c>
+      <c r="M2">
+        <v>2.718001771856228E-14</v>
+      </c>
+      <c r="N2">
+        <v>319989</v>
+      </c>
+      <c r="O2">
+        <v>1.520573672319186E-46</v>
+      </c>
+      <c r="P2">
+        <v>227435.5</v>
+      </c>
+      <c r="Q2">
+        <v>2.7100136505199899E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>150.8220466694533</v>
       </c>
       <c r="C3">
-        <v>150.8220466694533</v>
+        <v>1.7758598604935619E-33</v>
       </c>
       <c r="D3">
-        <v>1.7758598604935619E-33</v>
+        <v>229.81328397039741</v>
       </c>
       <c r="E3">
-        <v>229.81328397039741</v>
+        <v>1.4480640626053299E-48</v>
       </c>
       <c r="F3">
-        <v>1.4480640626053299E-48</v>
+        <v>420999</v>
       </c>
       <c r="G3">
-        <v>420999</v>
+        <v>1.710938413939372E-29</v>
       </c>
       <c r="H3">
-        <v>1.710938413939372E-29</v>
+        <v>329673</v>
+      </c>
+      <c r="I3">
+        <v>1.9788896998016131E-21</v>
+      </c>
+      <c r="J3">
+        <v>443807</v>
+      </c>
+      <c r="K3">
+        <v>0.38883258200001852</v>
+      </c>
+      <c r="L3">
+        <v>331098</v>
+      </c>
+      <c r="M3">
+        <v>4.9905244585054245E-10</v>
+      </c>
+      <c r="N3">
+        <v>326814</v>
+      </c>
+      <c r="O3">
+        <v>5.1271283921238008E-42</v>
+      </c>
+      <c r="P3">
+        <v>238660</v>
+      </c>
+      <c r="Q3">
+        <v>6.0701608258780668E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>75.077253054039829</v>
       </c>
       <c r="C4">
-        <v>75.077253054039829</v>
+        <v>4.9794530409933999E-17</v>
       </c>
       <c r="D4">
-        <v>4.9794530409933999E-17</v>
+        <v>83.883100735556582</v>
       </c>
       <c r="E4">
-        <v>83.883100735556582</v>
+        <v>2.61754304933234E-17</v>
       </c>
       <c r="F4">
-        <v>2.61754304933234E-17</v>
+        <v>357621</v>
       </c>
       <c r="G4">
-        <v>357621</v>
+        <v>2.5087458719708958E-11</v>
       </c>
       <c r="H4">
-        <v>2.5087458719708958E-11</v>
+        <v>263299</v>
+      </c>
+      <c r="I4">
+        <v>2.7562487332479849E-15</v>
+      </c>
+      <c r="J4">
+        <v>286424</v>
+      </c>
+      <c r="K4">
+        <v>0.1236930156564081</v>
+      </c>
+      <c r="L4">
+        <v>272550</v>
+      </c>
+      <c r="M4">
+        <v>4.8008739292989878E-7</v>
+      </c>
+      <c r="N4">
+        <v>292778</v>
+      </c>
+      <c r="O4">
+        <v>2.8979653490619891E-12</v>
+      </c>
+      <c r="P4">
+        <v>187487</v>
+      </c>
+      <c r="Q4">
+        <v>1.265966543206703E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>77.071299268967778</v>
       </c>
       <c r="C5">
-        <v>77.071299268967778</v>
+        <v>1.8372997129611001E-17</v>
       </c>
       <c r="D5">
-        <v>1.8372997129611001E-17</v>
+        <v>125.4235138372769</v>
       </c>
       <c r="E5">
-        <v>125.4235138372769</v>
+        <v>3.7055237499476162E-26</v>
       </c>
       <c r="F5">
-        <v>3.7055237499476162E-26</v>
+        <v>107010</v>
       </c>
       <c r="G5">
-        <v>107010</v>
+        <v>1.0208941484765571E-15</v>
       </c>
       <c r="H5">
-        <v>1.0208941484765571E-15</v>
+        <v>83068</v>
+      </c>
+      <c r="I5">
+        <v>4.4028115901363737E-12</v>
+      </c>
+      <c r="J5">
+        <v>116607</v>
+      </c>
+      <c r="K5">
+        <v>0.72550990873172472</v>
+      </c>
+      <c r="L5">
+        <v>71233</v>
+      </c>
+      <c r="M5">
+        <v>2.131289889380627E-10</v>
+      </c>
+      <c r="N5">
+        <v>84825</v>
+      </c>
+      <c r="O5">
+        <v>9.761379264539034E-24</v>
+      </c>
+      <c r="P5">
+        <v>55628</v>
+      </c>
+      <c r="Q5">
+        <v>7.1629967459187607E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>101.7846536397128</v>
       </c>
       <c r="C6">
-        <v>101.7846536397128</v>
+        <v>7.9021140031141892E-23</v>
       </c>
       <c r="D6">
-        <v>7.9021140031141892E-23</v>
+        <v>115.6031614179974</v>
       </c>
       <c r="E6">
-        <v>115.6031614179974</v>
+        <v>4.6396097644296492E-24</v>
       </c>
       <c r="F6">
-        <v>4.6396097644296492E-24</v>
+        <v>290671</v>
       </c>
       <c r="G6">
-        <v>290671</v>
+        <v>2.840560259325662E-18</v>
       </c>
       <c r="H6">
-        <v>2.840560259325662E-18</v>
+        <v>221819</v>
+      </c>
+      <c r="I6">
+        <v>2.632117984354202E-17</v>
+      </c>
+      <c r="J6">
+        <v>274797</v>
+      </c>
+      <c r="K6">
+        <v>0.75556874278776531</v>
+      </c>
+      <c r="L6">
+        <v>208840</v>
+      </c>
+      <c r="M6">
+        <v>4.9714609921689633E-12</v>
+      </c>
+      <c r="N6">
+        <v>239629</v>
+      </c>
+      <c r="O6">
+        <v>1.832423237886286E-19</v>
+      </c>
+      <c r="P6">
+        <v>150897</v>
+      </c>
+      <c r="Q6">
+        <v>1.1924736205481621E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>207.2223014091123</v>
       </c>
       <c r="C7">
-        <v>207.2223014091123</v>
+        <v>1.005191911679272E-45</v>
       </c>
       <c r="D7">
-        <v>1.005191911679272E-45</v>
+        <v>256.25490088807959</v>
       </c>
       <c r="E7">
-        <v>256.25490088807959</v>
+        <v>2.9239764335678902E-54</v>
       </c>
       <c r="F7">
-        <v>2.9239764335678902E-54</v>
+        <v>374249</v>
       </c>
       <c r="G7">
-        <v>374249</v>
+        <v>6.1505963230898775E-36</v>
       </c>
       <c r="H7">
-        <v>6.1505963230898775E-36</v>
+        <v>287985</v>
+      </c>
+      <c r="I7">
+        <v>9.8867144804845643E-33</v>
+      </c>
+      <c r="J7">
+        <v>380323</v>
+      </c>
+      <c r="K7">
+        <v>0.63065306812054056</v>
+      </c>
+      <c r="L7">
+        <v>314104</v>
+      </c>
+      <c r="M7">
+        <v>1.363731472170824E-13</v>
+      </c>
+      <c r="N7">
+        <v>295589</v>
+      </c>
+      <c r="O7">
+        <v>1.9380841514572239E-43</v>
+      </c>
+      <c r="P7">
+        <v>216476</v>
+      </c>
+      <c r="Q7">
+        <v>6.5821301207857419E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8">
+        <v>226.0450761962984</v>
       </c>
       <c r="C8">
-        <v>226.0450761962984</v>
+        <v>8.2212030232512655E-50</v>
       </c>
       <c r="D8">
-        <v>8.2212030232512655E-50</v>
+        <v>271.08260590029568</v>
       </c>
       <c r="E8">
-        <v>271.08260590029568</v>
+        <v>1.8639064087100169E-57</v>
       </c>
       <c r="F8">
-        <v>1.8639064087100169E-57</v>
+        <v>358063</v>
       </c>
       <c r="G8">
-        <v>358063</v>
+        <v>2.2856983346995119E-40</v>
       </c>
       <c r="H8">
-        <v>2.2856983346995119E-40</v>
+        <v>281644</v>
+      </c>
+      <c r="I8">
+        <v>5.8780431303140166E-34</v>
+      </c>
+      <c r="J8">
+        <v>381014</v>
+      </c>
+      <c r="K8">
+        <v>0.69291256417720393</v>
+      </c>
+      <c r="L8">
+        <v>298719</v>
+      </c>
+      <c r="M8">
+        <v>7.6988005402323547E-16</v>
+      </c>
+      <c r="N8">
+        <v>286595</v>
+      </c>
+      <c r="O8">
+        <v>2.089021552584996E-47</v>
+      </c>
+      <c r="P8">
+        <v>210915</v>
+      </c>
+      <c r="Q8">
+        <v>1.444193853364083E-5</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <v>252.12070930628761</v>
       </c>
       <c r="C9">
-        <v>252.12070930628761</v>
+        <v>1.7893017528224621E-55</v>
       </c>
       <c r="D9">
-        <v>1.7893017528224621E-55</v>
+        <v>347.21827680629758</v>
       </c>
       <c r="E9">
-        <v>347.21827680629758</v>
+        <v>6.9915932254672826E-74</v>
       </c>
       <c r="F9">
-        <v>6.9915932254672826E-74</v>
+        <v>536949</v>
       </c>
       <c r="G9">
-        <v>536949</v>
+        <v>6.5545926494945338E-43</v>
       </c>
       <c r="H9">
-        <v>6.5545926494945338E-43</v>
+        <v>407899</v>
+      </c>
+      <c r="I9">
+        <v>2.324850827288152E-40</v>
+      </c>
+      <c r="J9">
+        <v>562230</v>
+      </c>
+      <c r="K9">
+        <v>0.71931021559950281</v>
+      </c>
+      <c r="L9">
+        <v>423429</v>
+      </c>
+      <c r="M9">
+        <v>5.7489332674043724E-16</v>
+      </c>
+      <c r="N9">
+        <v>422793</v>
+      </c>
+      <c r="O9">
+        <v>7.1018383241337483E-59</v>
+      </c>
+      <c r="P9">
+        <v>304527</v>
+      </c>
+      <c r="Q9">
+        <v>9.0711601233876783E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>